<commit_message>
Remove classification_restrict to PCF
</commit_message>
<xml_diff>
--- a/abm/data/sbp_payments.xlsx
+++ b/abm/data/sbp_payments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\thesis-sbp-abm\municipality_level_analysis\municipalities_abm\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\sbp-adoption-abm\abm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059E5CFB-6E35-4633-809B-DF79CF38B2BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22711F8A-A3C2-4216-9F82-CD3949D5A689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,7 +367,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -511,8 +511,8 @@
         <v>2011</v>
       </c>
       <c r="B17" s="1">
-        <f>(38.94+43.58)/2+43.58+43.45</f>
-        <v>128.29000000000002</v>
+        <f>43.58+43.58+43.58</f>
+        <v>130.74</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>